<commit_message>
added options to handle date format
</commit_message>
<xml_diff>
--- a/LiveWatch/input_csvs/template/xangle_template_unlockschedule.xlsx
+++ b/LiveWatch/input_csvs/template/xangle_template_unlockschedule.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaewooklee/github/X-tools/LiveWatch/input_csvs/template/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jaewook.lee/github/X-tools/LiveWatch/input_csvs/template/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBE2D77A-B364-6048-B19C-04DA8F8DE9D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0060EF12-9255-8648-A1BB-0363665FC96F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{D774C16B-156A-426C-B083-1E59875B536B}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="28800" windowHeight="18000" xr2:uid="{D774C16B-156A-426C-B083-1E59875B536B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -467,8 +467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66A48455-4661-46EA-A947-AA5492862DB4}">
   <dimension ref="A1:B55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="F42" sqref="F42:F43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>